<commit_message>
Generative Summaries and Improved Topic Modelling, LLM classification for methods
</commit_message>
<xml_diff>
--- a/tables/section_counts.xlsx
+++ b/tables/section_counts.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -535,16 +535,6 @@
         <v>107</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" s="1" t="inlineStr">
-        <is>
-          <t>(2025, 2035]</t>
-        </is>
-      </c>
-      <c r="B11" t="n">
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Code Reformatting and Updated Figure 6
</commit_message>
<xml_diff>
--- a/tables/section_counts.xlsx
+++ b/tables/section_counts.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -448,100 +448,90 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>(1925, 1935]</t>
+          <t>(1935, 1945]</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>229</v>
+        <v>212</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>(1935, 1945]</t>
+          <t>(1945, 1955]</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>(1945, 1955]</t>
+          <t>(1955, 1965]</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>211</v>
+        <v>266</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>(1955, 1965]</t>
+          <t>(1965, 1975]</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>266</v>
+        <v>200</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>(1965, 1975]</t>
+          <t>(1975, 1985]</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>200</v>
+        <v>195</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>(1975, 1985]</t>
+          <t>(1985, 1995]</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>195</v>
+        <v>204</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>(1985, 1995]</t>
+          <t>(1995, 2005]</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>204</v>
+        <v>170</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>(1995, 2005]</t>
+          <t>(2005, 2015]</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>170</v>
+        <v>164</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>(2005, 2015]</t>
+          <t>(2015, 2025]</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="1" t="inlineStr">
-        <is>
-          <t>(2015, 2025]</t>
-        </is>
-      </c>
-      <c r="B11" t="n">
         <v>107</v>
       </c>
     </row>

</xml_diff>